<commit_message>
Update script and data
</commit_message>
<xml_diff>
--- a/dataImport.xlsx
+++ b/dataImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phucle/Projects/Psirenity/upload-icon-script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC012E75-240D-124B-9F64-D4A3D22845AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC5B2A3-EB79-FA40-A9FE-704545F6BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{84183BDE-2751-3341-ADAB-8E274F9DD420}"/>
   </bookViews>
@@ -35,42 +35,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>elegant-woman-lw-poly-silhouette.svg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>FILENAME</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>0_sitting-woman-silhouette-low-poly.svg</t>
+  </si>
+  <si>
+    <t>1_squirrel-silhouette-low-poly.svg</t>
+  </si>
+  <si>
+    <t>2_elegant-woman-lw-poly-silhouette.svg</t>
+  </si>
+  <si>
+    <t>3_spy-agent-silhouette.svg</t>
+  </si>
+  <si>
+    <t>4_fashionable-woman-low-poly.svg</t>
+  </si>
+  <si>
+    <t>fashionable-woman-low-poly</t>
+  </si>
+  <si>
+    <t>spy-agent-silhouette</t>
   </si>
   <si>
     <t>elegant-woman-lw-poly-silhouette</t>
   </si>
   <si>
-    <t>fashionable-woman-low-poly.svg</t>
-  </si>
-  <si>
-    <t>fashionable-woman-low-poly</t>
-  </si>
-  <si>
-    <t>sitting-woman-silhouette-low-poly.svg</t>
+    <t>squirrel-silhouette-low-poly</t>
   </si>
   <si>
     <t>sitting-woman-silhouette-low-poly</t>
-  </si>
-  <si>
-    <t>spy-agent-silhouette</t>
-  </si>
-  <si>
-    <t>spy-agent-silhouette.svg</t>
-  </si>
-  <si>
-    <t>squirrel-silhouette-low-poly.svg</t>
-  </si>
-  <si>
-    <t>FILENAME</t>
-  </si>
-  <si>
-    <t>CATEGORY</t>
-  </si>
-  <si>
-    <t>TAGS</t>
   </si>
 </sst>
 </file>
@@ -431,81 +434,81 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>